<commit_message>
Started added sample program for printing out results.
</commit_message>
<xml_diff>
--- a/Payslip.ConsoleApp/TimeSpent.xlsx
+++ b/Payslip.ConsoleApp/TimeSpent.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Stop</t>
   </si>
@@ -26,6 +26,12 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Learning about GIT</t>
   </si>
 </sst>
 </file>
@@ -369,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,7 +386,7 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -393,8 +399,11 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>42360</v>
       </c>
@@ -406,6 +415,20 @@
       </c>
       <c r="D2" s="1">
         <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>42369</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tests for PayPeriod formatting.
</commit_message>
<xml_diff>
--- a/Payslip.ConsoleApp/TimeSpent.xlsx
+++ b/Payslip.ConsoleApp/TimeSpent.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Stop</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Learning about GIT</t>
+  </si>
+  <si>
+    <t>Started added sample program for printing out results.</t>
   </si>
 </sst>
 </file>
@@ -375,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,6 +434,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.6875</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added IncomeTax to payslip.
</commit_message>
<xml_diff>
--- a/Payslip.ConsoleApp/TimeSpent.xlsx
+++ b/Payslip.ConsoleApp/TimeSpent.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Stop</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Started added sample program for printing out results.</t>
+  </si>
+  <si>
+    <t>Added pay period formatting.</t>
   </si>
 </sst>
 </file>
@@ -378,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,6 +448,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>42375</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Super to printout.
</commit_message>
<xml_diff>
--- a/Payslip.ConsoleApp/TimeSpent.xlsx
+++ b/Payslip.ConsoleApp/TimeSpent.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Stop</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Added pay period formatting.</t>
+  </si>
+  <si>
+    <t>Added income tax to payslip.</t>
   </si>
 </sst>
 </file>
@@ -381,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,6 +441,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>42369</v>
+      </c>
       <c r="B4" s="1">
         <v>0.66666666666666663</v>
       </c>
@@ -460,6 +466,20 @@
       </c>
       <c r="E5" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>42375</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.46875</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished reading payment startdate from CSV.
</commit_message>
<xml_diff>
--- a/Payslip.ConsoleApp/TimeSpent.xlsx
+++ b/Payslip.ConsoleApp/TimeSpent.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Stop</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Added income tax to payslip.</t>
+  </si>
+  <si>
+    <t>Finished funcationality.</t>
   </si>
 </sst>
 </file>
@@ -384,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,10 +479,24 @@
         <v>0.46875</v>
       </c>
       <c r="C6" s="1">
-        <v>0.48958333333333331</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>42376</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.5541666666666667</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>